<commit_message>
working on blank_set ru
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/zakaz.xlsx
+++ b/application/views/rpt/ru/doc/zakaz.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\isell3\application\views\rpt\ru\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
@@ -11,6 +16,9 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Лист1!$5:$5</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -21,57 +29,18 @@
     <t>№</t>
   </si>
   <si>
-    <t>Повна назва товару</t>
-  </si>
-  <si>
-    <t>К-ть</t>
-  </si>
-  <si>
-    <t>Цiна без ПДВ</t>
-  </si>
-  <si>
-    <t>Сума без ПДВ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Разом без ПДВ: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПДВ: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Всього з ПДВ: </t>
-  </si>
-  <si>
-    <t>Всього на суму:</t>
-  </si>
-  <si>
-    <t>Постачальник</t>
-  </si>
-  <si>
-    <t>Одержувач</t>
-  </si>
-  <si>
     <t>_____________________</t>
   </si>
   <si>
     <t>Артикул</t>
   </si>
   <si>
-    <t>Од. Вим</t>
-  </si>
-  <si>
     <t>{$v-&gt;p-&gt;all}</t>
   </si>
   <si>
     <t>{$v-&gt;a-&gt;all}</t>
   </si>
   <si>
-    <t>Замовлення товару № {$v-&gt;doc_view-&gt;view_num}</t>
-  </si>
-  <si>
-    <t>від {$v-&gt;doc_view-&gt;loc_date} р.</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;i}</t>
   </si>
   <si>
@@ -102,16 +71,55 @@
     <t>{$v-&gt;footer-&gt;total}</t>
   </si>
   <si>
-    <t>ПДВ: {$v-&gt;footer-&gt;vat}</t>
-  </si>
-  <si>
     <t>{$v-&gt;doc_view-&gt;total_spell}</t>
   </si>
   <si>
     <t>{$v-&gt;doc_view-&gt;user_sign}</t>
   </si>
   <si>
-    <t>Вага: {$v-&gt;footer-&gt;total_weight}кг Об`єм: {$v-&gt;footer-&gt;total_volume}м3</t>
+    <t>Заказ № {$v-&gt;doc_view-&gt;view_num}</t>
+  </si>
+  <si>
+    <t>от {$v-&gt;doc_view-&gt;loc_date} г.</t>
+  </si>
+  <si>
+    <t>Полное название товара</t>
+  </si>
+  <si>
+    <t>Ед. изм.</t>
+  </si>
+  <si>
+    <t>Кол-во</t>
+  </si>
+  <si>
+    <t>Цена без НДС</t>
+  </si>
+  <si>
+    <t>Сумма без НДС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Всего без НДС: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">НДС: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Всего с НДС: </t>
+  </si>
+  <si>
+    <t>Всего на сумму:</t>
+  </si>
+  <si>
+    <t>НДС: {$v-&gt;footer-&gt;vat}</t>
+  </si>
+  <si>
+    <t>Вес: {$v-&gt;footer-&gt;total_weight}кг Объем: {$v-&gt;footer-&gt;total_volume}м3</t>
+  </si>
+  <si>
+    <t>Поставщик</t>
+  </si>
+  <si>
+    <t>Получатель</t>
   </si>
 </sst>
 </file>
@@ -296,6 +304,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -303,33 +338,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -340,6 +348,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -388,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,172 +646,172 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="A1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="A4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="11"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="11"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -809,43 +820,48 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="17"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="17"/>
+      <c r="F13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="A16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="F13:G13"/>
@@ -857,13 +873,8 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:G3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>